<commit_message>
created oat envelope labels csv
</commit_message>
<xml_diff>
--- a/data/PM3D_trial.xlsx
+++ b/data/PM3D_trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\B4I\B4I_hyde\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464146F9-E8A2-455C-A680-F98B2F92CE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C865E89F-CCC6-477D-BC49-67AE81BC35A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{0DBC6980-D01B-44B4-B932-6965585E0927}"/>
   </bookViews>
@@ -1521,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3394EE7F-7A70-4202-9F3B-60629FBFAD0A}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,12 +1532,14 @@
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>276</v>
       </c>
@@ -1566,585 +1568,479 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7">
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="7">
+        <v>102</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>103.3</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1">
-        <v>60</v>
-      </c>
-      <c r="G3" s="1">
-        <v>67.599999999999994</v>
-      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="7">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>274</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="7">
+        <v>202</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1">
-        <v>60</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" s="7">
         <v>1</v>
       </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="7">
+        <v>201</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>274</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1">
-        <v>60</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5" s="7">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7">
+        <v>301</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1">
-        <v>62</v>
-      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I6" s="7">
         <v>1</v>
       </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="7">
+        <v>302</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>94</v>
-      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I7" s="7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="7">
+        <v>402</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1">
-        <v>24</v>
-      </c>
-      <c r="G8" s="1">
-        <v>56.4</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="7">
+        <v>401</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>82.5</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="7">
+        <v>4</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7">
+        <v>501</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="7">
         <v>5</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="1">
-        <v>24</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7">
-        <v>9</v>
-      </c>
       <c r="I10" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10</v>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="7">
+        <v>502</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="1">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1">
-        <v>56.4</v>
-      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I11" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="1">
-        <v>11</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="7">
+        <v>602</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>112.7</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I12" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="7">
+        <v>601</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="1">
-        <v>24</v>
-      </c>
-      <c r="G13" s="1">
-        <v>67.599999999999994</v>
-      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I13" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="1">
-        <v>13</v>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="7">
+        <v>701</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="1">
-        <v>24</v>
-      </c>
-      <c r="G14" s="1">
-        <v>56.1</v>
-      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I14" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="7">
+        <v>702</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1">
-        <v>24</v>
-      </c>
-      <c r="G15" s="1">
-        <v>62</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I15" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="1">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>6</v>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="7">
+        <v>802</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>93.5</v>
-      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I16" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="1">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>274</v>
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="7">
+        <v>801</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="1">
-        <v>60</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
       <c r="H17" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I17" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>17</v>
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="7">
+        <v>901</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="1">
-        <v>24</v>
-      </c>
-      <c r="G18" s="1">
-        <v>49.5</v>
-      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="7">
+        <v>9</v>
+      </c>
+      <c r="I18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="7">
+        <v>902</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="7">
+        <v>9</v>
+      </c>
+      <c r="I19" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1002</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1">
-        <v>24</v>
-      </c>
-      <c r="G19" s="1">
-        <v>56.1</v>
-      </c>
-      <c r="H19" s="7">
-        <v>8</v>
-      </c>
-      <c r="I19" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="1">
-        <v>24</v>
-      </c>
-      <c r="G20" s="1">
-        <v>49.5</v>
-      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I20" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="1">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1001</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>274</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="1">
-        <v>60</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
       <c r="H21" s="7">
         <v>10</v>
       </c>
@@ -2427,7 +2323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
@@ -2452,7 +2348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>37</v>
       </c>
@@ -2477,7 +2373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
@@ -2502,7 +2398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -2527,7 +2423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
@@ -2552,7 +2448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
@@ -2577,7 +2473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>37</v>
       </c>
@@ -2602,7 +2498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
@@ -2627,7 +2523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
@@ -2652,479 +2548,585 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="7">
-        <v>101</v>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>103.3</v>
+      </c>
+      <c r="H42" s="7">
+        <v>1</v>
+      </c>
+      <c r="I42" s="7">
+        <v>1</v>
+      </c>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="7">
-        <v>1</v>
-      </c>
-      <c r="I42" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="7">
-        <v>102</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="F43" s="1">
+        <v>60</v>
+      </c>
+      <c r="G43" s="1">
+        <v>67.599999999999994</v>
+      </c>
       <c r="H43" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="7">
-        <v>202</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="8" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="F44" s="1">
+        <v>60</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
       <c r="H44" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I44" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="7">
-        <v>201</v>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="1">
+        <v>4</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="1">
+        <v>60</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="7">
+        <v>4</v>
+      </c>
+      <c r="I45" s="7">
+        <v>1</v>
+      </c>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="1">
         <v>5</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="7">
-        <v>2</v>
-      </c>
-      <c r="I45" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="7">
-        <v>301</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="F46" s="1">
+        <v>24</v>
+      </c>
+      <c r="G46" s="1">
+        <v>62</v>
+      </c>
       <c r="H46" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I46" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="7">
-        <v>302</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="1"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="1">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>94</v>
+      </c>
       <c r="H47" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I47" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="7">
-        <v>402</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="1">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E48" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="F48" s="1">
+        <v>24</v>
+      </c>
+      <c r="G48" s="1">
+        <v>56.4</v>
+      </c>
       <c r="H48" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I48" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="7">
-        <v>401</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="1"/>
+      <c r="A49" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="1">
+        <v>8</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>82.5</v>
+      </c>
       <c r="H49" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I49" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B50" s="7">
-        <v>501</v>
+      <c r="A50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1">
+        <v>9</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="1">
+        <v>24</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="7">
         <v>9</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="7">
-        <v>5</v>
-      </c>
       <c r="I50" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" s="7">
-        <v>502</v>
+      <c r="A51" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="1">
+        <v>10</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="F51" s="1">
+        <v>24</v>
+      </c>
+      <c r="G51" s="1">
+        <v>56.4</v>
+      </c>
       <c r="H51" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I51" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="7">
-        <v>602</v>
+      <c r="A52" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="1">
+        <v>11</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>112.7</v>
+      </c>
       <c r="H52" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I52" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="7">
-        <v>601</v>
+      <c r="A53" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="1">
+        <v>12</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="F53" s="1">
+        <v>24</v>
+      </c>
+      <c r="G53" s="1">
+        <v>67.599999999999994</v>
+      </c>
       <c r="H53" s="7">
+        <v>2</v>
+      </c>
+      <c r="I53" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="1">
+        <v>13</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I53" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="7">
-        <v>701</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+      <c r="F54" s="1">
+        <v>24</v>
+      </c>
+      <c r="G54" s="1">
+        <v>56.1</v>
+      </c>
       <c r="H54" s="7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I54" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="7">
-        <v>702</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="1"/>
+      <c r="A55" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="1">
+        <v>14</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="F55" s="1">
+        <v>24</v>
+      </c>
+      <c r="G55" s="1">
+        <v>62</v>
+      </c>
       <c r="H55" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I55" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="7">
-        <v>802</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="8" t="s">
-        <v>2</v>
+      <c r="A56" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="1">
+        <v>15</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>93.5</v>
+      </c>
       <c r="H56" s="7">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I56" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" s="7">
-        <v>801</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="8" t="s">
-        <v>8</v>
+      <c r="A57" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="1">
+        <v>16</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="F57" s="1">
+        <v>60</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
       <c r="H57" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I57" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B58" s="7">
-        <v>901</v>
+      <c r="A58" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="1">
+        <v>17</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="F58" s="1">
+        <v>24</v>
+      </c>
+      <c r="G58" s="1">
+        <v>49.5</v>
+      </c>
       <c r="H58" s="7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I58" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B59" s="7">
-        <v>902</v>
-      </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="8" t="s">
-        <v>10</v>
+      <c r="A59" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="1">
+        <v>18</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="1">
+        <v>24</v>
+      </c>
+      <c r="G59" s="1">
+        <v>56.1</v>
+      </c>
+      <c r="H59" s="7">
+        <v>8</v>
+      </c>
+      <c r="I59" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="1">
         <v>19</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="7">
-        <v>9</v>
-      </c>
-      <c r="I59" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" s="7">
-        <v>1002</v>
-      </c>
       <c r="C60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
+      <c r="F60" s="1">
+        <v>24</v>
+      </c>
+      <c r="G60" s="1">
+        <v>49.5</v>
+      </c>
       <c r="H60" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I60" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B61" s="7">
-        <v>1001</v>
-      </c>
-      <c r="C61" s="8" t="s">
+      <c r="A61" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="1">
+        <v>20</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="1"/>
+      <c r="D61" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="E61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="F61" s="1">
+        <v>60</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
       <c r="H61" s="7">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
added envelop script, added AI layout fieldbook merge
</commit_message>
<xml_diff>
--- a/data/PM3D_trial.xlsx
+++ b/data/PM3D_trial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\B4I\B4I_hyde\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4878D777-090D-4F14-98C8-34BAA148A5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D8CFBE-5447-4721-8B1F-ECD89AAB095F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="2775" windowWidth="25065" windowHeight="17115" activeTab="1" xr2:uid="{0DBC6980-D01B-44B4-B932-6965585E0927}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{0DBC6980-D01B-44B4-B932-6965585E0927}"/>
   </bookViews>
   <sheets>
     <sheet name="seed envelop " sheetId="1" r:id="rId1"/>
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,8 +1517,8 @@
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>